<commit_message>
feat: (user) login functionality
</commit_message>
<xml_diff>
--- a/db/seeds/excel/seeds.xlsx
+++ b/db/seeds/excel/seeds.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -505,14 +505,14 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="29.796875"/>
-    <col customWidth="true" max="2" min="2" width="13.9296875"/>
-    <col customWidth="true" max="4" min="4" width="72.6640625"/>
+    <col min="1" max="1" width="29.796875" customWidth="1"/>
+    <col min="2" max="2" width="13.9296875" customWidth="1"/>
+    <col min="4" max="4" width="72.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -523,7 +523,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -552,14 +552,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27"/>
-    <col customWidth="true" max="2" min="2" width="18.19921875"/>
-    <col customWidth="true" max="3" min="3" width="69.796875"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" customWidth="1"/>
+    <col min="3" max="3" width="69.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -570,7 +570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -591,14 +591,14 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="28.6640625"/>
-    <col customWidth="true" max="2" min="2" width="14.06640625"/>
-    <col customWidth="true" max="4" min="4" width="70.796875"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.06640625" customWidth="1"/>
+    <col min="4" max="4" width="70.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -612,7 +612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -633,7 +633,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>